<commit_message>
Added last 2 days prior to harvest to csv file
</commit_message>
<xml_diff>
--- a/Lysimetry+Info.xlsx
+++ b/Lysimetry+Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Desktop\Demorie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demoriegalarza/Desktop/DFD+DAG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F1EE67-8B9C-4494-9352-F53B5F43722E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8F65C0-43DC-6B46-8F5B-D7B660D612A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8835" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A3CF4042-8C22-5346-88AF-41094BEDD8CE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="17460" windowHeight="14040" xr2:uid="{A3CF4042-8C22-5346-88AF-41094BEDD8CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Harvest Days" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="124">
   <si>
     <t>NM31</t>
   </si>
@@ -391,6 +391,24 @@
   </si>
   <si>
     <t>08/10/23</t>
+  </si>
+  <si>
+    <t>LastDay1</t>
+  </si>
+  <si>
+    <t>LastDay2</t>
+  </si>
+  <si>
+    <t>07/05/23</t>
+  </si>
+  <si>
+    <t>07/23/23</t>
+  </si>
+  <si>
+    <t>08/14/23</t>
+  </si>
+  <si>
+    <t>07/11/23</t>
   </si>
 </sst>
 </file>
@@ -451,57 +469,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="20">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -808,6 +790,45 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -822,39 +843,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5D9A6B68-7201-4C61-8E7E-E4E48D246456}" name="Table2" displayName="Table2" ref="A1:B82" totalsRowShown="0">
-  <autoFilter ref="A1:B82" xr:uid="{5D9A6B68-7201-4C61-8E7E-E4E48D246456}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7DBC6D1A-9712-45E6-8C81-65CDAC979259}" name="Sample" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{01BDD02C-153F-4149-A568-286081A2DDEA}" name="HarvestDate" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5D9A6B68-7201-4C61-8E7E-E4E48D246456}" name="Table2" displayName="Table2" ref="A1:D82" totalsRowShown="0">
+  <autoFilter ref="A1:D82" xr:uid="{5D9A6B68-7201-4C61-8E7E-E4E48D246456}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C82">
+    <sortCondition ref="A1:A82"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{7DBC6D1A-9712-45E6-8C81-65CDAC979259}" name="Sample" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{01BDD02C-153F-4149-A568-286081A2DDEA}" name="HarvestDate" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{EE7095DE-6A0A-F64A-A8A4-95379EDC12B4}" name="LastDay1"/>
+    <tableColumn id="4" xr3:uid="{5CC3F3B9-D4E9-EC4A-8F3F-7872190E2AEC}" name="LastDay2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEC0B367-E6C2-4259-BB2A-9677B93597CC}" name="Table1" displayName="Table1" ref="A1:P90" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEC0B367-E6C2-4259-BB2A-9677B93597CC}" name="Table1" displayName="Table1" ref="A1:P90" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A1:P90" xr:uid="{DEC0B367-E6C2-4259-BB2A-9677B93597CC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P90">
     <sortCondition ref="P1:P90"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{22ED5F58-E21D-43DD-85BD-D7581091CAFA}" name="ID" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{40824ACA-85BA-45DB-A84E-1A28EAF050A9}" name="06/23/2023" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{77C00E66-C350-4B11-869B-277D41A627F2}" name="06/26/23" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{1A52CB7F-5A53-45EC-B33D-ABBAF7C3A849}" name="06/29/23" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{67E6BD79-B0FB-4FB0-8433-45688D4FB5AF}" name="07/03/23" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{84085F5E-4164-4E2B-9B2D-856227BA361B}" name="07/06/23" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{02AF54B9-B11F-4856-B40A-246C736597C0}" name="07/10/23" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{82424F3D-158B-4405-93D0-062E22130AA6}" name="07/13/23" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{C23E27D8-3846-44D6-827B-F64D60D38385}" name="07/17/23" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{ACE08182-835E-4D24-9A9A-82A5690A2D31}" name="07/20/23" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{711661E6-E5C2-4E4C-BFF4-3622F3DFB78E}" name="07/24/23" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{16690697-7004-4EBA-9E97-429E46A2A56B}" name="07/27/23" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{209EE87A-29BB-465C-A972-352695ADF915}" name="07/31/23" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{C4834610-39C1-4A06-88BC-4BC4BAE8D7AC}" name="08/03/23" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{AD5EA7C0-0A73-42E4-B0BE-F78A32F59861}" name="08/07/23" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{1BAEFA27-EC75-47D6-88A3-C3C8E6F5620F}" name="08/10/23" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{22ED5F58-E21D-43DD-85BD-D7581091CAFA}" name="ID" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{40824ACA-85BA-45DB-A84E-1A28EAF050A9}" name="06/23/2023" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{77C00E66-C350-4B11-869B-277D41A627F2}" name="06/26/23" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{1A52CB7F-5A53-45EC-B33D-ABBAF7C3A849}" name="06/29/23" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{67E6BD79-B0FB-4FB0-8433-45688D4FB5AF}" name="07/03/23" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{84085F5E-4164-4E2B-9B2D-856227BA361B}" name="07/06/23" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{02AF54B9-B11F-4856-B40A-246C736597C0}" name="07/10/23" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{82424F3D-158B-4405-93D0-062E22130AA6}" name="07/13/23" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{C23E27D8-3846-44D6-827B-F64D60D38385}" name="07/17/23" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{ACE08182-835E-4D24-9A9A-82A5690A2D31}" name="07/20/23" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{711661E6-E5C2-4E4C-BFF4-3622F3DFB78E}" name="07/24/23" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{16690697-7004-4EBA-9E97-429E46A2A56B}" name="07/27/23" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{209EE87A-29BB-465C-A972-352695ADF915}" name="07/31/23" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{C4834610-39C1-4A06-88BC-4BC4BAE8D7AC}" name="08/03/23" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{AD5EA7C0-0A73-42E4-B0BE-F78A32F59861}" name="08/07/23" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{1BAEFA27-EC75-47D6-88A3-C3C8E6F5620F}" name="08/10/23" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1179,678 +1205,1164 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D513E18-DFCF-024B-BDA7-D7C3EF458E2A}">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B82"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79:D79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.75" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>100</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="C1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="C2" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+        <v>56</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+        <v>28</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+        <v>81</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+        <v>72</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+        <v>49</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="C13" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>106</v>
+      </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="C15" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="4" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="4" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+        <v>99</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+        <v>97</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+        <v>96</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+        <v>94</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+        <v>98</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+        <v>90</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+        <v>98</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+        <v>2</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A31" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="4" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A32" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A33" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+        <v>95</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+        <v>97</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+        <v>98</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C38" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+        <v>93</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+        <v>91</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+        <v>95</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+        <v>93</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+        <v>99</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B44" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+        <v>90</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
+        <v>97</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
+        <v>5</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
+        <v>99</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
+        <v>92</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
+        <v>91</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C51" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B52" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A53" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A54" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A55" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A56" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A57" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A58" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58" s="4" t="s">
+      <c r="C62" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A59" s="1" t="s">
+      <c r="C69" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A60" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A61" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A62" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A63" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A64" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A65" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A66" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A67" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A68" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A69" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A70" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A71" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A72" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C72" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>79</v>
+        <v>9</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.4">
+        <v>90</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C74" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.4">
+        <v>95</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>82</v>
+        <v>31</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.4">
+        <v>93</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.4">
+        <v>98</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.4">
+        <v>96</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A80" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C80" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.4">
+        <v>6</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>99</v>
+        <v>91</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1866,13 +2378,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6B19627-F820-7B46-B36F-5DDD5EE9A757}">
   <dimension ref="A1:P90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.75" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
@@ -1888,7 +2400,7 @@
     <col min="16" max="16" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>108</v>
       </c>
@@ -1938,7 +2450,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>81</v>
       </c>
@@ -1988,7 +2500,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>72</v>
       </c>
@@ -2038,7 +2550,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>84</v>
       </c>
@@ -2088,7 +2600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>79</v>
       </c>
@@ -2138,7 +2650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>80</v>
       </c>
@@ -2188,7 +2700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>73</v>
       </c>
@@ -2238,7 +2750,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>76</v>
       </c>
@@ -2288,7 +2800,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>75</v>
       </c>
@@ -2338,7 +2850,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>83</v>
       </c>
@@ -2388,7 +2900,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>86</v>
       </c>
@@ -2438,7 +2950,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>74</v>
       </c>
@@ -2488,7 +3000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>78</v>
       </c>
@@ -2538,7 +3050,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>87</v>
       </c>
@@ -2588,7 +3100,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>88</v>
       </c>
@@ -2638,7 +3150,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>82</v>
       </c>
@@ -2688,7 +3200,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>77</v>
       </c>
@@ -2738,7 +3250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>85</v>
       </c>
@@ -2788,7 +3300,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>56</v>
       </c>
@@ -2836,7 +3348,7 @@
       </c>
       <c r="P19" s="2"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>62</v>
       </c>
@@ -2884,7 +3396,7 @@
       </c>
       <c r="P20" s="2"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>58</v>
       </c>
@@ -2932,7 +3444,7 @@
       </c>
       <c r="P21" s="2"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>60</v>
       </c>
@@ -2980,7 +3492,7 @@
       </c>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>61</v>
       </c>
@@ -3028,7 +3540,7 @@
       </c>
       <c r="P23" s="2"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>59</v>
       </c>
@@ -3076,7 +3588,7 @@
       </c>
       <c r="P24" s="2"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>63</v>
       </c>
@@ -3124,7 +3636,7 @@
       </c>
       <c r="P25" s="2"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>57</v>
       </c>
@@ -3172,7 +3684,7 @@
       </c>
       <c r="P26" s="2"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>64</v>
       </c>
@@ -3218,7 +3730,7 @@
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>65</v>
       </c>
@@ -3264,7 +3776,7 @@
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>69</v>
       </c>
@@ -3310,7 +3822,7 @@
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>66</v>
       </c>
@@ -3356,7 +3868,7 @@
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>70</v>
       </c>
@@ -3402,7 +3914,7 @@
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>71</v>
       </c>
@@ -3448,7 +3960,7 @@
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>67</v>
       </c>
@@ -3494,7 +4006,7 @@
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>68</v>
       </c>
@@ -3540,7 +4052,7 @@
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>48</v>
       </c>
@@ -3584,7 +4096,7 @@
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>42</v>
       </c>
@@ -3628,7 +4140,7 @@
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>45</v>
       </c>
@@ -3672,7 +4184,7 @@
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
@@ -3716,7 +4228,7 @@
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
@@ -3760,7 +4272,7 @@
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>47</v>
       </c>
@@ -3804,7 +4316,7 @@
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>44</v>
       </c>
@@ -3848,7 +4360,7 @@
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>49</v>
       </c>
@@ -3890,7 +4402,7 @@
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>50</v>
       </c>
@@ -3932,7 +4444,7 @@
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>53</v>
       </c>
@@ -3974,7 +4486,7 @@
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>51</v>
       </c>
@@ -4016,7 +4528,7 @@
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>55</v>
       </c>
@@ -4058,7 +4570,7 @@
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>54</v>
       </c>
@@ -4100,7 +4612,7 @@
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>52</v>
       </c>
@@ -4142,7 +4654,7 @@
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>28</v>
       </c>
@@ -4182,7 +4694,7 @@
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>30</v>
       </c>
@@ -4222,7 +4734,7 @@
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>29</v>
       </c>
@@ -4262,7 +4774,7 @@
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>33</v>
       </c>
@@ -4302,7 +4814,7 @@
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>34</v>
       </c>
@@ -4342,7 +4854,7 @@
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>32</v>
       </c>
@@ -4382,7 +4894,7 @@
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>31</v>
       </c>
@@ -4422,7 +4934,7 @@
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>35</v>
       </c>
@@ -4460,7 +4972,7 @@
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>37</v>
       </c>
@@ -4498,7 +5010,7 @@
       <c r="O57" s="2"/>
       <c r="P57" s="2"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>39</v>
       </c>
@@ -4536,7 +5048,7 @@
       <c r="O58" s="2"/>
       <c r="P58" s="2"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>38</v>
       </c>
@@ -4574,7 +5086,7 @@
       <c r="O59" s="2"/>
       <c r="P59" s="2"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>36</v>
       </c>
@@ -4612,7 +5124,7 @@
       <c r="O60" s="2"/>
       <c r="P60" s="2"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>41</v>
       </c>
@@ -4650,7 +5162,7 @@
       <c r="O61" s="2"/>
       <c r="P61" s="2"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>40</v>
       </c>
@@ -4688,7 +5200,7 @@
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>14</v>
       </c>
@@ -4724,7 +5236,7 @@
       <c r="O63" s="2"/>
       <c r="P63" s="2"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>15</v>
       </c>
@@ -4760,7 +5272,7 @@
       <c r="O64" s="2"/>
       <c r="P64" s="2"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>18</v>
       </c>
@@ -4796,7 +5308,7 @@
       <c r="O65" s="2"/>
       <c r="P65" s="2"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>16</v>
       </c>
@@ -4832,7 +5344,7 @@
       <c r="O66" s="2"/>
       <c r="P66" s="2"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>20</v>
       </c>
@@ -4868,7 +5380,7 @@
       <c r="O67" s="2"/>
       <c r="P67" s="2"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>17</v>
       </c>
@@ -4904,7 +5416,7 @@
       <c r="O68" s="2"/>
       <c r="P68" s="2"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>19</v>
       </c>
@@ -4940,7 +5452,7 @@
       <c r="O69" s="2"/>
       <c r="P69" s="2"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>22</v>
       </c>
@@ -4974,7 +5486,7 @@
       <c r="O70" s="2"/>
       <c r="P70" s="2"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>21</v>
       </c>
@@ -5008,7 +5520,7 @@
       <c r="O71" s="2"/>
       <c r="P71" s="2"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>27</v>
       </c>
@@ -5042,7 +5554,7 @@
       <c r="O72" s="2"/>
       <c r="P72" s="2"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>26</v>
       </c>
@@ -5076,7 +5588,7 @@
       <c r="O73" s="2"/>
       <c r="P73" s="2"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>24</v>
       </c>
@@ -5110,7 +5622,7 @@
       <c r="O74" s="2"/>
       <c r="P74" s="2"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>23</v>
       </c>
@@ -5144,7 +5656,7 @@
       <c r="O75" s="2"/>
       <c r="P75" s="2"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>25</v>
       </c>
@@ -5178,7 +5690,7 @@
       <c r="O76" s="2"/>
       <c r="P76" s="2"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>4</v>
       </c>
@@ -5210,7 +5722,7 @@
       <c r="O77" s="2"/>
       <c r="P77" s="2"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>0</v>
       </c>
@@ -5242,7 +5754,7 @@
       <c r="O78" s="2"/>
       <c r="P78" s="2"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>2</v>
       </c>
@@ -5274,7 +5786,7 @@
       <c r="O79" s="2"/>
       <c r="P79" s="2"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>3</v>
       </c>
@@ -5306,7 +5818,7 @@
       <c r="O80" s="2"/>
       <c r="P80" s="2"/>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>5</v>
       </c>
@@ -5338,7 +5850,7 @@
       <c r="O81" s="2"/>
       <c r="P81" s="2"/>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>1</v>
       </c>
@@ -5370,7 +5882,7 @@
       <c r="O82" s="2"/>
       <c r="P82" s="2"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>6</v>
       </c>
@@ -5402,7 +5914,7 @@
       <c r="O83" s="2"/>
       <c r="P83" s="2"/>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>8</v>
       </c>
@@ -5432,7 +5944,7 @@
       <c r="O84" s="2"/>
       <c r="P84" s="2"/>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>7</v>
       </c>
@@ -5462,7 +5974,7 @@
       <c r="O85" s="2"/>
       <c r="P85" s="2"/>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>12</v>
       </c>
@@ -5492,7 +6004,7 @@
       <c r="O86" s="2"/>
       <c r="P86" s="2"/>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>11</v>
       </c>
@@ -5522,7 +6034,7 @@
       <c r="O87" s="2"/>
       <c r="P87" s="2"/>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>13</v>
       </c>
@@ -5552,7 +6064,7 @@
       <c r="O88" s="2"/>
       <c r="P88" s="2"/>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>9</v>
       </c>
@@ -5582,7 +6094,7 @@
       <c r="O89" s="2"/>
       <c r="P89" s="2"/>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Added columns for time difference
</commit_message>
<xml_diff>
--- a/Lysimetry+Info.xlsx
+++ b/Lysimetry+Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demoriegalarza/Desktop/DFD+DAG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8F65C0-43DC-6B46-8F5B-D7B660D612A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D404723-C409-0D42-ABAD-4A58078B9275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="17460" windowHeight="14040" xr2:uid="{A3CF4042-8C22-5346-88AF-41094BEDD8CE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="17460" windowHeight="14040" activeTab="1" xr2:uid="{A3CF4042-8C22-5346-88AF-41094BEDD8CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Harvest Days" sheetId="1" r:id="rId1"/>
@@ -345,9 +345,6 @@
     <t>HarvestDate</t>
   </si>
   <si>
-    <t>06/23/2023</t>
-  </si>
-  <si>
     <t>06/26/23</t>
   </si>
   <si>
@@ -409,6 +406,9 @@
   </si>
   <si>
     <t>07/11/23</t>
+  </si>
+  <si>
+    <t>06/23/23</t>
   </si>
 </sst>
 </file>
@@ -866,7 +866,7 @@
   </sortState>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{22ED5F58-E21D-43DD-85BD-D7581091CAFA}" name="ID" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{40824ACA-85BA-45DB-A84E-1A28EAF050A9}" name="06/23/2023" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{40824ACA-85BA-45DB-A84E-1A28EAF050A9}" name="06/23/23" dataDxfId="14"/>
     <tableColumn id="3" xr3:uid="{77C00E66-C350-4B11-869B-277D41A627F2}" name="06/26/23" dataDxfId="13"/>
     <tableColumn id="4" xr3:uid="{1A52CB7F-5A53-45EC-B33D-ABBAF7C3A849}" name="06/29/23" dataDxfId="12"/>
     <tableColumn id="5" xr3:uid="{67E6BD79-B0FB-4FB0-8433-45688D4FB5AF}" name="07/03/23" dataDxfId="11"/>
@@ -1205,7 +1205,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D513E18-DFCF-024B-BDA7-D7C3EF458E2A}">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C79" sqref="C79:D79"/>
     </sheetView>
   </sheetViews>
@@ -1224,10 +1224,10 @@
         <v>101</v>
       </c>
       <c r="C1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" t="s">
         <v>118</v>
-      </c>
-      <c r="D1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1238,10 +1238,10 @@
         <v>89</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1252,10 +1252,10 @@
         <v>97</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1266,10 +1266,10 @@
         <v>93</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1280,7 +1280,7 @@
         <v>99</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>98</v>
@@ -1294,10 +1294,10 @@
         <v>98</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1308,7 +1308,7 @@
         <v>96</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>95</v>
@@ -1322,10 +1322,10 @@
         <v>91</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1336,10 +1336,10 @@
         <v>95</v>
       </c>
       <c r="C9" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1350,7 +1350,7 @@
         <v>99</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>98</v>
@@ -1364,7 +1364,7 @@
         <v>94</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>93</v>
@@ -1378,10 +1378,10 @@
         <v>91</v>
       </c>
       <c r="C12" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1392,10 +1392,10 @@
         <v>90</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1406,10 +1406,10 @@
         <v>89</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -1421,10 +1421,10 @@
         <v>90</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1435,10 +1435,10 @@
         <v>97</v>
       </c>
       <c r="C16" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1449,7 +1449,7 @@
         <v>92</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>91</v>
@@ -1463,10 +1463,10 @@
         <v>95</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1477,10 +1477,10 @@
         <v>98</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1491,7 +1491,7 @@
         <v>92</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>91</v>
@@ -1505,7 +1505,7 @@
         <v>92</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>91</v>
@@ -1519,7 +1519,7 @@
         <v>99</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>98</v>
@@ -1533,10 +1533,10 @@
         <v>97</v>
       </c>
       <c r="C23" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1547,7 +1547,7 @@
         <v>96</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>95</v>
@@ -1561,7 +1561,7 @@
         <v>94</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>93</v>
@@ -1575,10 +1575,10 @@
         <v>98</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1589,10 +1589,10 @@
         <v>90</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1603,10 +1603,10 @@
         <v>98</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1617,10 +1617,10 @@
         <v>89</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1631,7 +1631,7 @@
         <v>96</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>95</v>
@@ -1645,7 +1645,7 @@
         <v>94</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>93</v>
@@ -1659,10 +1659,10 @@
         <v>90</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1673,7 +1673,7 @@
         <v>94</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>93</v>
@@ -1687,10 +1687,10 @@
         <v>95</v>
       </c>
       <c r="C34" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1701,10 +1701,10 @@
         <v>89</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1715,10 +1715,10 @@
         <v>97</v>
       </c>
       <c r="C36" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1729,10 +1729,10 @@
         <v>98</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1743,7 +1743,7 @@
         <v>94</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>93</v>
@@ -1757,10 +1757,10 @@
         <v>93</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1771,10 +1771,10 @@
         <v>91</v>
       </c>
       <c r="C40" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D40" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1785,10 +1785,10 @@
         <v>95</v>
       </c>
       <c r="C41" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1799,10 +1799,10 @@
         <v>93</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1813,7 +1813,7 @@
         <v>99</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>98</v>
@@ -1827,7 +1827,7 @@
         <v>96</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>95</v>
@@ -1841,10 +1841,10 @@
         <v>90</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1855,10 +1855,10 @@
         <v>97</v>
       </c>
       <c r="C46" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1869,10 +1869,10 @@
         <v>89</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1883,7 +1883,7 @@
         <v>99</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>98</v>
@@ -1897,7 +1897,7 @@
         <v>92</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>91</v>
@@ -1911,10 +1911,10 @@
         <v>91</v>
       </c>
       <c r="C50" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1925,7 +1925,7 @@
         <v>96</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>95</v>
@@ -1939,10 +1939,10 @@
         <v>89</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1953,10 +1953,10 @@
         <v>95</v>
       </c>
       <c r="C53" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D53" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1967,10 +1967,10 @@
         <v>90</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1981,7 +1981,7 @@
         <v>92</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D55" s="7" t="s">
         <v>91</v>
@@ -1995,10 +1995,10 @@
         <v>98</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -2009,10 +2009,10 @@
         <v>97</v>
       </c>
       <c r="C57" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D57" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -2023,10 +2023,10 @@
         <v>95</v>
       </c>
       <c r="C58" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -2037,7 +2037,7 @@
         <v>94</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D59" s="7" t="s">
         <v>93</v>
@@ -2051,10 +2051,10 @@
         <v>98</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -2065,7 +2065,7 @@
         <v>99</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>98</v>
@@ -2079,7 +2079,7 @@
         <v>96</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>95</v>
@@ -2093,7 +2093,7 @@
         <v>92</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>91</v>
@@ -2107,10 +2107,10 @@
         <v>93</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -2121,10 +2121,10 @@
         <v>91</v>
       </c>
       <c r="C65" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D65" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2135,7 +2135,7 @@
         <v>94</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>93</v>
@@ -2149,10 +2149,10 @@
         <v>91</v>
       </c>
       <c r="C67" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D67" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2163,7 +2163,7 @@
         <v>99</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>98</v>
@@ -2177,10 +2177,10 @@
         <v>97</v>
       </c>
       <c r="C69" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D69" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2191,10 +2191,10 @@
         <v>93</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2205,10 +2205,10 @@
         <v>93</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2219,10 +2219,10 @@
         <v>97</v>
       </c>
       <c r="C72" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D72" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -2233,10 +2233,10 @@
         <v>90</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -2247,7 +2247,7 @@
         <v>99</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>98</v>
@@ -2261,10 +2261,10 @@
         <v>95</v>
       </c>
       <c r="C75" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D75" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2275,10 +2275,10 @@
         <v>93</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2289,10 +2289,10 @@
         <v>98</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2303,7 +2303,7 @@
         <v>96</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>95</v>
@@ -2317,7 +2317,7 @@
         <v>92</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D79" s="7" t="s">
         <v>91</v>
@@ -2331,7 +2331,7 @@
         <v>99</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>98</v>
@@ -2345,10 +2345,10 @@
         <v>89</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -2359,10 +2359,10 @@
         <v>91</v>
       </c>
       <c r="C82" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D82" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="D82" s="7" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2378,8 +2378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6B19627-F820-7B46-B36F-5DDD5EE9A757}">
   <dimension ref="A1:P90"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2402,52 +2402,52 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
New scripts for Figures and Stats
</commit_message>
<xml_diff>
--- a/Lysimetry+Info.xlsx
+++ b/Lysimetry+Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demoriegalarza/Desktop/DFD+DAG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7FE419-CEBE-A64C-8B4B-E9D040C7196E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93464DF-1135-1C44-AF48-5F8022FA850B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13260" yWindow="500" windowWidth="12340" windowHeight="14040" xr2:uid="{A3CF4042-8C22-5346-88AF-41094BEDD8CE}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Days Watered" sheetId="3" r:id="rId2"/>
     <sheet name="Days Measured" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="161">
   <si>
     <t>NM31</t>
   </si>
@@ -518,6 +518,9 @@
   </si>
   <si>
     <t>Day0</t>
+  </si>
+  <si>
+    <t>08/09/23</t>
   </si>
 </sst>
 </file>
@@ -576,7 +579,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -584,51 +587,41 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF44B3E1"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF44B3E1"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF44B3E1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="23">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     </dxf>
@@ -957,9 +950,6 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -997,10 +987,10 @@
     <sortCondition ref="A1:A90"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7DBC6D1A-9712-45E6-8C81-65CDAC979259}" name="ID" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{01BDD02C-153F-4149-A568-286081A2DDEA}" name="HarvestDate" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{EE7095DE-6A0A-F64A-A8A4-95379EDC12B4}" name="LastDay1"/>
-    <tableColumn id="4" xr3:uid="{5CC3F3B9-D4E9-EC4A-8F3F-7872190E2AEC}" name="LastDay2"/>
+    <tableColumn id="1" xr3:uid="{7DBC6D1A-9712-45E6-8C81-65CDAC979259}" name="ID" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{01BDD02C-153F-4149-A568-286081A2DDEA}" name="HarvestDate" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{EE7095DE-6A0A-F64A-A8A4-95379EDC12B4}" name="LastDay1" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{5CC3F3B9-D4E9-EC4A-8F3F-7872190E2AEC}" name="LastDay2" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{68D286CD-10E6-1847-94D4-97EBE91DAF02}" name="Day0" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1008,28 +998,28 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEC0B367-E6C2-4259-BB2A-9677B93597CC}" name="Table1" displayName="Table1" ref="A1:P90" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEC0B367-E6C2-4259-BB2A-9677B93597CC}" name="Table1" displayName="Table1" ref="A1:P90" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:P90" xr:uid="{DEC0B367-E6C2-4259-BB2A-9677B93597CC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P90">
     <sortCondition ref="P1:P90"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{22ED5F58-E21D-43DD-85BD-D7581091CAFA}" name="ID" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{40824ACA-85BA-45DB-A84E-1A28EAF050A9}" name="06/23/23" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{77C00E66-C350-4B11-869B-277D41A627F2}" name="06/26/23" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{1A52CB7F-5A53-45EC-B33D-ABBAF7C3A849}" name="06/29/23" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{67E6BD79-B0FB-4FB0-8433-45688D4FB5AF}" name="07/03/23" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{84085F5E-4164-4E2B-9B2D-856227BA361B}" name="07/06/23" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{02AF54B9-B11F-4856-B40A-246C736597C0}" name="07/10/23" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{82424F3D-158B-4405-93D0-062E22130AA6}" name="07/13/23" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{C23E27D8-3846-44D6-827B-F64D60D38385}" name="07/17/23" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{ACE08182-835E-4D24-9A9A-82A5690A2D31}" name="07/20/23" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{711661E6-E5C2-4E4C-BFF4-3622F3DFB78E}" name="07/24/23" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{16690697-7004-4EBA-9E97-429E46A2A56B}" name="07/27/23" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{209EE87A-29BB-465C-A972-352695ADF915}" name="07/31/23" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{C4834610-39C1-4A06-88BC-4BC4BAE8D7AC}" name="08/03/23" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{AD5EA7C0-0A73-42E4-B0BE-F78A32F59861}" name="08/07/23" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{1BAEFA27-EC75-47D6-88A3-C3C8E6F5620F}" name="08/10/23" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{22ED5F58-E21D-43DD-85BD-D7581091CAFA}" name="ID" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{40824ACA-85BA-45DB-A84E-1A28EAF050A9}" name="06/23/23" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{77C00E66-C350-4B11-869B-277D41A627F2}" name="06/26/23" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{1A52CB7F-5A53-45EC-B33D-ABBAF7C3A849}" name="06/29/23" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{67E6BD79-B0FB-4FB0-8433-45688D4FB5AF}" name="07/03/23" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{84085F5E-4164-4E2B-9B2D-856227BA361B}" name="07/06/23" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{02AF54B9-B11F-4856-B40A-246C736597C0}" name="07/10/23" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{82424F3D-158B-4405-93D0-062E22130AA6}" name="07/13/23" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{C23E27D8-3846-44D6-827B-F64D60D38385}" name="07/17/23" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{ACE08182-835E-4D24-9A9A-82A5690A2D31}" name="07/20/23" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{711661E6-E5C2-4E4C-BFF4-3622F3DFB78E}" name="07/24/23" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{16690697-7004-4EBA-9E97-429E46A2A56B}" name="07/27/23" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{209EE87A-29BB-465C-A972-352695ADF915}" name="07/31/23" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{C4834610-39C1-4A06-88BC-4BC4BAE8D7AC}" name="08/03/23" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{AD5EA7C0-0A73-42E4-B0BE-F78A32F59861}" name="08/07/23" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{1BAEFA27-EC75-47D6-88A3-C3C8E6F5620F}" name="08/10/23" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1355,31 +1345,32 @@
   <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="5"/>
+    <col min="5" max="5" width="10.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1387,1442 +1378,1383 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E5" s="9">
-        <v>45148</v>
+      <c r="E5" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="E6" s="9">
-        <v>45148</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E7" s="9">
-        <v>45134</v>
+      <c r="E7" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E10" s="9">
-        <v>45148</v>
+      <c r="E10" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="14">
-        <v>45147</v>
-      </c>
-      <c r="C11" s="15">
-        <v>45145</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="B11" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E11" s="9">
-        <v>45141</v>
+      <c r="E11" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E12" s="9">
-        <v>45127</v>
+      <c r="E12" s="5" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E14" s="9">
-        <v>45113</v>
+      <c r="E14" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E15" s="12"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E16" s="9">
-        <v>45113</v>
+      <c r="E16" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E18" s="9">
-        <v>45120</v>
+      <c r="E18" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="14">
-        <v>45147</v>
-      </c>
-      <c r="C20" s="15">
-        <v>45145</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="B20" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E20" s="9">
-        <v>45141</v>
+      <c r="E20" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="E21" s="9">
-        <v>45148</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E22" s="9">
-        <v>45120</v>
+      <c r="E22" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="13">
-        <v>45120</v>
+      <c r="E23" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E24" s="9">
-        <v>45148</v>
+      <c r="E24" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E26" s="9">
-        <v>45134</v>
+      <c r="E26" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="9">
-        <v>45127</v>
+      <c r="E27" s="5" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="E28" s="9">
-        <v>45148</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="14">
-        <v>45147</v>
-      </c>
-      <c r="C29" s="15">
-        <v>45145</v>
-      </c>
-      <c r="D29" s="4" t="s">
+      <c r="B29" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E29" s="9">
-        <v>45141</v>
+      <c r="E29" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E30" s="9">
-        <v>45113</v>
+      <c r="E30" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="E31" s="9">
-        <v>45148</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E32" s="9"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E33" s="9">
-        <v>45134</v>
+      <c r="E33" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="14">
-        <v>45147</v>
-      </c>
-      <c r="C34" s="15">
-        <v>45145</v>
-      </c>
-      <c r="D34" s="4" t="s">
+      <c r="B34" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E34" s="9">
-        <v>45141</v>
+      <c r="E34" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E35" s="9">
-        <v>45127</v>
+      <c r="E35" s="5" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E36" s="9">
-        <v>45113</v>
+      <c r="E36" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E37" s="9">
-        <v>45127</v>
+      <c r="E37" s="5" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E38" s="9"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E39" s="9"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="E40" s="9"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="E41" s="9">
-        <v>45148</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E42" s="9">
-        <v>45127</v>
+      <c r="E42" s="5" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E43" s="9"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E44" s="9"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E45" s="9"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E46" s="9"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E47" s="9">
-        <v>45148</v>
+      <c r="E47" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E48" s="9">
-        <v>45134</v>
+      <c r="E48" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E49" s="13">
-        <v>45113</v>
+      <c r="E49" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="E50" s="9"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E51" s="9"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C52" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E52" s="9">
-        <v>45148</v>
+      <c r="E52" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E53" s="13">
-        <v>45120</v>
+      <c r="E53" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E54" s="9"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E55" s="13">
-        <v>45134</v>
+      <c r="E55" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C56" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E56" s="9"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C57" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E57" s="9"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C58" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E58" s="9">
-        <v>45113</v>
+      <c r="E58" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E59" s="13">
-        <v>45120</v>
+      <c r="E59" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="E60" s="9">
-        <v>45148</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="E61" s="9"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B62" s="14">
-        <v>45147</v>
-      </c>
-      <c r="C62" s="15">
-        <v>45145</v>
-      </c>
-      <c r="D62" s="4" t="s">
+      <c r="B62" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D62" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E62" s="9">
-        <v>45141</v>
+      <c r="E62" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C63" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E63" s="9"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C64" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E64" s="13">
-        <v>45127</v>
+      <c r="E64" s="5" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C65" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D65" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="E65" s="9">
-        <v>45148</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C66" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D66" s="7" t="s">
+      <c r="D66" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E66" s="9">
-        <v>45148</v>
+      <c r="E66" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="C67" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D67" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E67" s="9">
-        <v>45134</v>
+      <c r="E67" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="14">
-        <v>45147</v>
-      </c>
-      <c r="C68" s="15">
-        <v>45145</v>
-      </c>
-      <c r="D68" s="4" t="s">
+      <c r="B68" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D68" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E68" s="9">
-        <v>45141</v>
+      <c r="E68" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C69" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D69" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E69" s="13">
-        <v>45120</v>
+      <c r="E69" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C70" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D70" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E70" s="9"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="C71" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D71" s="7" t="s">
+      <c r="D71" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E71" s="9"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="C72" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D72" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E72" s="9">
-        <v>45127</v>
+      <c r="E72" s="5" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C73" s="8" t="s">
+      <c r="C73" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D73" s="7" t="s">
+      <c r="D73" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E73" s="9"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C74" s="7" t="s">
+      <c r="C74" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D74" s="7" t="s">
+      <c r="D74" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E74" s="9">
-        <v>45148</v>
+      <c r="E74" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C75" s="7" t="s">
+      <c r="C75" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D75" s="7" t="s">
+      <c r="D75" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="E75" s="9"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C76" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D76" s="7" t="s">
+      <c r="D76" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E76" s="9"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C77" s="7" t="s">
+      <c r="C77" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D77" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E77" s="9"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C78" s="7" t="s">
+      <c r="C78" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D78" s="7" t="s">
+      <c r="D78" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="E78" s="9"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="C79" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D79" s="7" t="s">
+      <c r="D79" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E79" s="13">
-        <v>45113</v>
+      <c r="E79" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C80" s="7" t="s">
+      <c r="C80" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D80" s="7" t="s">
+      <c r="D80" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E80" s="9">
-        <v>45148</v>
+      <c r="E80" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C81" s="7" t="s">
+      <c r="C81" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="D81" s="7" t="s">
+      <c r="D81" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E81" s="9"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B82" s="14">
-        <v>45147</v>
-      </c>
-      <c r="C82" s="15">
-        <v>45145</v>
-      </c>
-      <c r="D82" s="4" t="s">
+      <c r="B82" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D82" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E82" s="9">
-        <v>45141</v>
+      <c r="E82" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B83" s="14">
-        <v>45147</v>
-      </c>
-      <c r="C83" s="15">
-        <v>45145</v>
-      </c>
-      <c r="D83" s="4" t="s">
+      <c r="B83" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D83" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E83" s="9">
-        <v>45141</v>
+      <c r="E83" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C84" s="7" t="s">
+      <c r="C84" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D84" s="7" t="s">
+      <c r="D84" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E84" s="9"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="C85" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D85" s="7" t="s">
+      <c r="D85" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="E85" s="9">
-        <v>45148</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C86" s="7" t="s">
+      <c r="C86" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D86" s="7" t="s">
+      <c r="D86" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E86" s="9">
-        <v>45134</v>
+      <c r="E86" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C87" s="7" t="s">
+      <c r="C87" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D87" s="7" t="s">
+      <c r="D87" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E87" s="13">
-        <v>45120</v>
+      <c r="E87" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="C88" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D88" s="7" t="s">
+      <c r="D88" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E88" s="9">
-        <v>45148</v>
+      <c r="E88" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C89" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D89" s="7" t="s">
+      <c r="D89" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E89" s="9"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C90" s="8" t="s">
+      <c r="C90" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D90" s="7" t="s">
+      <c r="D90" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="E90" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -2864,49 +2796,49 @@
       <c r="A1" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>115</v>
       </c>
     </row>
@@ -6607,16 +6539,16 @@
     <col min="2" max="2" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="11" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:2" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="7" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="9">
+      <c r="A2" s="5">
         <v>45098</v>
       </c>
       <c r="B2" t="s">
@@ -6624,7 +6556,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
+      <c r="A3" s="5">
         <v>45099</v>
       </c>
       <c r="B3" t="s">
@@ -6632,7 +6564,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
+      <c r="A4" s="5">
         <v>45100</v>
       </c>
       <c r="B4" t="s">
@@ -6640,7 +6572,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
+      <c r="A5" s="5">
         <v>45103</v>
       </c>
       <c r="B5" t="s">
@@ -6648,7 +6580,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="9">
+      <c r="A6" s="5">
         <v>45104</v>
       </c>
       <c r="B6" t="s">
@@ -6656,7 +6588,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="9">
+      <c r="A7" s="5">
         <v>45105</v>
       </c>
       <c r="B7" t="s">
@@ -6664,7 +6596,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
+      <c r="A8" s="5">
         <v>45106</v>
       </c>
       <c r="B8" t="s">
@@ -6672,7 +6604,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="9">
+      <c r="A9" s="5">
         <v>45110</v>
       </c>
       <c r="B9" t="s">
@@ -6680,7 +6612,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
+      <c r="A10" s="5">
         <v>45112</v>
       </c>
       <c r="B10" t="s">
@@ -6688,7 +6620,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
+      <c r="A11" s="5">
         <v>45113</v>
       </c>
       <c r="B11" t="s">
@@ -6696,7 +6628,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
+      <c r="A12" s="5">
         <v>45114</v>
       </c>
       <c r="B12" t="s">
@@ -6704,7 +6636,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
+      <c r="A13" s="5">
         <v>45117</v>
       </c>
       <c r="B13" t="s">
@@ -6712,7 +6644,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="9">
+      <c r="A14" s="5">
         <v>45118</v>
       </c>
       <c r="B14" t="s">
@@ -6720,7 +6652,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
+      <c r="A15" s="5">
         <v>45119</v>
       </c>
       <c r="B15" t="s">
@@ -6728,7 +6660,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
+      <c r="A16" s="5">
         <v>45120</v>
       </c>
       <c r="B16" t="s">
@@ -6736,7 +6668,7 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
+      <c r="A17" s="5">
         <v>45124</v>
       </c>
       <c r="B17" t="s">
@@ -6744,7 +6676,7 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
+      <c r="A18" s="5">
         <v>45125</v>
       </c>
       <c r="B18" t="s">
@@ -6752,7 +6684,7 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" s="9">
+      <c r="A19" s="5">
         <v>45126</v>
       </c>
       <c r="B19" t="s">
@@ -6760,30 +6692,30 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="9">
+      <c r="A20" s="5">
         <v>45127</v>
       </c>
       <c r="B20" t="s">
         <v>143</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" s="9">
+      <c r="A21" s="5">
         <v>45131</v>
       </c>
       <c r="B21" t="s">
@@ -6791,7 +6723,7 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" s="9">
+      <c r="A22" s="5">
         <v>45132</v>
       </c>
       <c r="B22" t="s">
@@ -6799,7 +6731,7 @@
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" s="9">
+      <c r="A23" s="5">
         <v>45133</v>
       </c>
       <c r="B23" t="s">
@@ -6807,7 +6739,7 @@
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" s="9">
+      <c r="A24" s="5">
         <v>45134</v>
       </c>
       <c r="B24" t="s">
@@ -6815,7 +6747,7 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="9">
+      <c r="A25" s="5">
         <v>45138</v>
       </c>
       <c r="B25" t="s">
@@ -6823,7 +6755,7 @@
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" s="9">
+      <c r="A26" s="5">
         <v>45139</v>
       </c>
       <c r="B26" t="s">
@@ -6831,7 +6763,7 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27" s="9">
+      <c r="A27" s="5">
         <v>45140</v>
       </c>
       <c r="B27" t="s">
@@ -6839,7 +6771,7 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A28" s="9">
+      <c r="A28" s="5">
         <v>45141</v>
       </c>
       <c r="B28" t="s">
@@ -6847,7 +6779,7 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A29" s="9">
+      <c r="A29" s="5">
         <v>45145</v>
       </c>
       <c r="B29" t="s">
@@ -6855,7 +6787,7 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30" s="9">
+      <c r="A30" s="5">
         <v>45146</v>
       </c>
       <c r="B30" t="s">
@@ -6863,7 +6795,7 @@
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A31" s="9">
+      <c r="A31" s="5">
         <v>45147</v>
       </c>
       <c r="B31" t="s">
@@ -6871,7 +6803,7 @@
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32" s="9">
+      <c r="A32" s="5">
         <v>45148</v>
       </c>
       <c r="B32" t="s">
@@ -6879,7 +6811,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="9">
+      <c r="A33" s="5">
         <v>45152</v>
       </c>
       <c r="B33" t="s">
@@ -6887,7 +6819,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="9">
+      <c r="A34" s="5">
         <v>45153</v>
       </c>
       <c r="B34" t="s">
@@ -6895,7 +6827,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="9">
+      <c r="A35" s="5">
         <v>45154</v>
       </c>
       <c r="B35" t="s">
@@ -6903,7 +6835,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
+      <c r="A39" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
New scripts for Figured and Stats
</commit_message>
<xml_diff>
--- a/Lysimetry+Info.xlsx
+++ b/Lysimetry+Info.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demoriegalarza/Desktop/DFD+DAG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93464DF-1135-1C44-AF48-5F8022FA850B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12C2B58-8BB0-9C4C-BC0F-D3DCD0D16B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13260" yWindow="500" windowWidth="12340" windowHeight="14040" xr2:uid="{A3CF4042-8C22-5346-88AF-41094BEDD8CE}"/>
+    <workbookView xWindow="8260" yWindow="500" windowWidth="17340" windowHeight="14040" activeTab="1" xr2:uid="{A3CF4042-8C22-5346-88AF-41094BEDD8CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Harvest Days" sheetId="1" r:id="rId1"/>
-    <sheet name="Days Watered" sheetId="3" r:id="rId2"/>
-    <sheet name="Days Measured" sheetId="4" r:id="rId3"/>
+    <sheet name="Difference" sheetId="5" r:id="rId2"/>
+    <sheet name="Days Watered" sheetId="3" r:id="rId3"/>
+    <sheet name="Days Measured" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="161">
   <si>
     <t>NM31</t>
   </si>
@@ -591,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -608,23 +609,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -950,6 +940,18 @@
       </font>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -988,38 +990,38 @@
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{7DBC6D1A-9712-45E6-8C81-65CDAC979259}" name="ID" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{01BDD02C-153F-4149-A568-286081A2DDEA}" name="HarvestDate" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{EE7095DE-6A0A-F64A-A8A4-95379EDC12B4}" name="LastDay1" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{5CC3F3B9-D4E9-EC4A-8F3F-7872190E2AEC}" name="LastDay2" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{68D286CD-10E6-1847-94D4-97EBE91DAF02}" name="Day0" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{01BDD02C-153F-4149-A568-286081A2DDEA}" name="HarvestDate" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{EE7095DE-6A0A-F64A-A8A4-95379EDC12B4}" name="LastDay1" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{5CC3F3B9-D4E9-EC4A-8F3F-7872190E2AEC}" name="LastDay2" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{68D286CD-10E6-1847-94D4-97EBE91DAF02}" name="Day0" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEC0B367-E6C2-4259-BB2A-9677B93597CC}" name="Table1" displayName="Table1" ref="A1:P90" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DEC0B367-E6C2-4259-BB2A-9677B93597CC}" name="Table1" displayName="Table1" ref="A1:P90" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A1:P90" xr:uid="{DEC0B367-E6C2-4259-BB2A-9677B93597CC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P90">
     <sortCondition ref="P1:P90"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{22ED5F58-E21D-43DD-85BD-D7581091CAFA}" name="ID" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{40824ACA-85BA-45DB-A84E-1A28EAF050A9}" name="06/23/23" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{77C00E66-C350-4B11-869B-277D41A627F2}" name="06/26/23" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{1A52CB7F-5A53-45EC-B33D-ABBAF7C3A849}" name="06/29/23" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{67E6BD79-B0FB-4FB0-8433-45688D4FB5AF}" name="07/03/23" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{84085F5E-4164-4E2B-9B2D-856227BA361B}" name="07/06/23" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{02AF54B9-B11F-4856-B40A-246C736597C0}" name="07/10/23" dataDxfId="13"/>
-    <tableColumn id="8" xr3:uid="{82424F3D-158B-4405-93D0-062E22130AA6}" name="07/13/23" dataDxfId="12"/>
-    <tableColumn id="9" xr3:uid="{C23E27D8-3846-44D6-827B-F64D60D38385}" name="07/17/23" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{ACE08182-835E-4D24-9A9A-82A5690A2D31}" name="07/20/23" dataDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{711661E6-E5C2-4E4C-BFF4-3622F3DFB78E}" name="07/24/23" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{16690697-7004-4EBA-9E97-429E46A2A56B}" name="07/27/23" dataDxfId="8"/>
-    <tableColumn id="13" xr3:uid="{209EE87A-29BB-465C-A972-352695ADF915}" name="07/31/23" dataDxfId="7"/>
-    <tableColumn id="14" xr3:uid="{C4834610-39C1-4A06-88BC-4BC4BAE8D7AC}" name="08/03/23" dataDxfId="6"/>
-    <tableColumn id="15" xr3:uid="{AD5EA7C0-0A73-42E4-B0BE-F78A32F59861}" name="08/07/23" dataDxfId="5"/>
-    <tableColumn id="16" xr3:uid="{1BAEFA27-EC75-47D6-88A3-C3C8E6F5620F}" name="08/10/23" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{22ED5F58-E21D-43DD-85BD-D7581091CAFA}" name="ID" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{40824ACA-85BA-45DB-A84E-1A28EAF050A9}" name="06/23/23" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{77C00E66-C350-4B11-869B-277D41A627F2}" name="06/26/23" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{1A52CB7F-5A53-45EC-B33D-ABBAF7C3A849}" name="06/29/23" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{67E6BD79-B0FB-4FB0-8433-45688D4FB5AF}" name="07/03/23" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{84085F5E-4164-4E2B-9B2D-856227BA361B}" name="07/06/23" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{02AF54B9-B11F-4856-B40A-246C736597C0}" name="07/10/23" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{82424F3D-158B-4405-93D0-062E22130AA6}" name="07/13/23" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{C23E27D8-3846-44D6-827B-F64D60D38385}" name="07/17/23" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{ACE08182-835E-4D24-9A9A-82A5690A2D31}" name="07/20/23" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{711661E6-E5C2-4E4C-BFF4-3622F3DFB78E}" name="07/24/23" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{16690697-7004-4EBA-9E97-429E46A2A56B}" name="07/27/23" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{209EE87A-29BB-465C-A972-352695ADF915}" name="07/31/23" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{C4834610-39C1-4A06-88BC-4BC4BAE8D7AC}" name="08/03/23" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{AD5EA7C0-0A73-42E4-B0BE-F78A32F59861}" name="08/07/23" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{1BAEFA27-EC75-47D6-88A3-C3C8E6F5620F}" name="08/10/23" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1344,8 +1346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D513E18-DFCF-024B-BDA7-D7C3EF458E2A}">
   <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2766,11 +2768,537 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB4207CD-3E0C-0949-9E9A-8B466AF86500}">
+  <dimension ref="A1:C46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="131" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6B19627-F820-7B46-B36F-5DDD5EE9A757}">
   <dimension ref="A1:P90"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="125" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+    <sheetView zoomScale="125" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A2" sqref="A2:XFD18"/>
     </sheetView>
   </sheetViews>
@@ -6524,7 +7052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D715E13-8C4E-594F-8579-9FA3FA0EC40F}">
   <dimension ref="A1:Q39"/>
   <sheetViews>

</xml_diff>